<commit_message>
upload dicionario de dados base
upload dicionario de dados base
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_dados.xlsx
+++ b/dicionario_dados/dicionario_dados.xlsx
@@ -1,42 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur_pc\Documents\arthur\GitHub\StoreStocker\dicionario_dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cristoffer.187823\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFCEC26-2E8A-4825-951A-0DF577DE660D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15615" windowHeight="7680" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="saldoestoque" sheetId="1" r:id="rId1"/>
     <sheet name="item" sheetId="2" r:id="rId2"/>
+    <sheet name="entradasaida" sheetId="3" r:id="rId3"/>
+    <sheet name="moviestoque" sheetId="4" r:id="rId4"/>
+    <sheet name="tipomov" sheetId="5" r:id="rId5"/>
+    <sheet name="documento" sheetId="6" r:id="rId6"/>
+    <sheet name="venda" sheetId="7" r:id="rId7"/>
+    <sheet name="status" sheetId="8" r:id="rId8"/>
+    <sheet name="categoria" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="103">
   <si>
     <t>Tabela</t>
   </si>
@@ -119,9 +116,6 @@
     <t>quantidade</t>
   </si>
   <si>
-    <t>0 - sem limite</t>
-  </si>
-  <si>
     <t>Coluna com a quantidade de peças no estoque</t>
   </si>
   <si>
@@ -192,12 +186,168 @@
   </si>
   <si>
     <t>idx_id_item</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>0 - 2.147.483.647</t>
+  </si>
+  <si>
+    <t>id_entrada_saida</t>
+  </si>
+  <si>
+    <t>entrada_saida_nome</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>entradasaida</t>
+  </si>
+  <si>
+    <t>moviestoque</t>
+  </si>
+  <si>
+    <t>id_movimentacao</t>
+  </si>
+  <si>
+    <t>dentificador único da movimentação de estoque.</t>
+  </si>
+  <si>
+    <t>id_tipo_mov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t>id_documento</t>
+  </si>
+  <si>
+    <t>data_movi</t>
+  </si>
+  <si>
+    <t>time_stamp</t>
+  </si>
+  <si>
+    <t>Referência ao item movimentado.</t>
+  </si>
+  <si>
+    <t>Tipo de movimentação (entrada ou saída).</t>
+  </si>
+  <si>
+    <t>Referência ao tipo de entrada/saída</t>
+  </si>
+  <si>
+    <t>Referência ao documento que originou a movimentação.</t>
+  </si>
+  <si>
+    <t>Quantidade movimentada</t>
+  </si>
+  <si>
+    <t>Data da movimentação</t>
+  </si>
+  <si>
+    <t>tipomov</t>
+  </si>
+  <si>
+    <t>Identificador único do tipo de movimentação.</t>
+  </si>
+  <si>
+    <t>Nome do tipo de movimentação (entrada ou saída).</t>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>tipo_nome</t>
+  </si>
+  <si>
+    <t>documento</t>
+  </si>
+  <si>
+    <t>Identificador único do documento.</t>
+  </si>
+  <si>
+    <t>Tipo de entrada/saída relacionado ao documento.</t>
+  </si>
+  <si>
+    <t>motivo_balanco</t>
+  </si>
+  <si>
+    <t>Motivo da baixa no estoque (se aplicável).</t>
+  </si>
+  <si>
+    <t>numero_nota</t>
+  </si>
+  <si>
+    <t>id_venda</t>
+  </si>
+  <si>
+    <t>Referência à venda associada ao documento.</t>
+  </si>
+  <si>
+    <t>Número da nota fiscal (se aplicável).</t>
+  </si>
+  <si>
+    <t>VARCHAR(200)</t>
+  </si>
+  <si>
+    <t>venda</t>
+  </si>
+  <si>
+    <t>nome_cliente</t>
+  </si>
+  <si>
+    <t>metodo_pagamento</t>
+  </si>
+  <si>
+    <t>Identificador único da venda.</t>
+  </si>
+  <si>
+    <t>Nome do cliente da venda.</t>
+  </si>
+  <si>
+    <t>Método de pagamento utilizado na venda.</t>
+  </si>
+  <si>
+    <t>VARCHAR(30)</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>status_nome</t>
+  </si>
+  <si>
+    <t>VARCHAR(15)</t>
+  </si>
+  <si>
+    <t>Nome do status (ativo ou desativado).</t>
+  </si>
+  <si>
+    <t>Identificador único do status.</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>Identificador único da categoria.</t>
+  </si>
+  <si>
+    <t>Nome da categoria de item.</t>
+  </si>
+  <si>
+    <t>VARCHAR(20)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -312,6 +462,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -338,6 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,11 +808,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H11" sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,47 +826,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -730,16 +887,14 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
@@ -752,15 +907,15 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
+      <c r="D6" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>9</v>
@@ -774,15 +929,15 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
+      <c r="D7" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
@@ -790,12 +945,12 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -804,22 +959,22 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
@@ -829,17 +984,17 @@
       <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="10"/>
+      <c r="A11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="12"/>
       <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
@@ -852,8 +1007,8 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -883,11 +1038,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,47 +1057,47 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="B2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
@@ -963,12 +1118,12 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="6" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>23</v>
@@ -985,12 +1140,12 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="D6" s="6">
         <v>100</v>
@@ -1001,16 +1156,16 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3">
         <v>300</v>
@@ -1021,16 +1176,16 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D8" s="3">
         <v>8.1999999999999993</v>
@@ -1041,16 +1196,16 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="14"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3">
         <v>15</v>
@@ -1059,32 +1214,32 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="14"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1099,19 +1254,19 @@
         <v>24</v>
       </c>
       <c r="H11" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>9</v>
@@ -1121,12 +1276,12 @@
         <v>24</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1136,22 +1291,22 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="11"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1161,17 +1316,17 @@
       <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="10"/>
+      <c r="A16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="12"/>
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
@@ -1184,8 +1339,8 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1195,6 +1350,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -1207,14 +1368,1512 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D078EF7-3BBE-41A4-99BD-8D8B99FF2FFE}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="10">
+        <v>50</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED20376C-1613-4C04-B236-53AD0407EF67}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="13"/>
+      <c r="C13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7CFD9F-9919-4B0B-BC86-D4D4925DE626}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E06F406-FB9E-4E77-9906-55508E8DD12C}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="10">
+        <v>200</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6702861-0CC5-44FB-ADD9-CA5AA23D8CF9}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="10">
+        <v>100</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="10">
+        <v>30</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632521AC-016F-40FD-B467-57DCF009FA1A}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="10">
+        <v>15</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90865C74-AEB8-4A50-9C23-4D48804F86FA}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="10">
+        <v>20</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>